<commit_message>
restore 3 omitted buildings
</commit_message>
<xml_diff>
--- a/buildings_demographics.xlsx
+++ b/buildings_demographics.xlsx
@@ -10,12 +10,9 @@
     <sheet name="buildings_demographics" sheetId="1" r:id="rId1"/>
     <sheet name="buildings_demographics_clean" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">buildings_demographics!$A$1:$N$721</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">buildings_demographics_clean!$A$1:$O$318</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">buildings_demographics!$A$1:$N$720</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">buildings_demographics_clean!$A$1:$O$317</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -4672,22 +4669,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="tableau"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="countDistinct"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4976,11 +4957,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N721"/>
+  <dimension ref="A1:N720"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A569" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D665" sqref="D665"/>
+      <pane ySplit="1" topLeftCell="A710" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A721" sqref="A721:XFD721"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36551,38 +36532,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="721" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A721">
-        <f>[1]!countDistinct(A2:A720)</f>
-        <v>719</v>
-      </c>
-      <c r="C721">
-        <f>[1]!countDistinct(C2:C720)</f>
-        <v>313</v>
-      </c>
-      <c r="D721">
-        <f>[1]!countDistinct(D2:D720)</f>
-        <v>338</v>
-      </c>
-      <c r="F721">
-        <f>[1]!countDistinct(F2:F720)</f>
-        <v>338</v>
-      </c>
-      <c r="G721">
-        <f>[1]!countDistinct(G2:G720)</f>
-        <v>311</v>
-      </c>
-      <c r="H721">
-        <f>[1]!countDistinct(H2:H720)</f>
-        <v>315</v>
-      </c>
-      <c r="J721">
-        <f>[1]!countDistinct(J2:J720)</f>
-        <v>338</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:N721">
+  <autoFilter ref="A1:N720">
     <filterColumn colId="4">
       <filters blank="1">
         <filter val="Academic &amp; Admin: Large"/>
@@ -36607,11 +36558,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O318"/>
+  <dimension ref="A1:O317"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A318" sqref="A318:XFD318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51783,18 +51734,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D318">
-        <f>[1]!countDistinct(D2:D317)</f>
-        <v>316</v>
-      </c>
-      <c r="E318">
-        <f>[1]!countDistinct(E1:E317)</f>
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:O318"/>
+  <autoFilter ref="A1:O317"/>
   <sortState ref="A107:O274">
     <sortCondition ref="D2:D274"/>
   </sortState>

</xml_diff>